<commit_message>
Update documentation of loguniform
</commit_message>
<xml_diff>
--- a/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
+++ b/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\src\semeio\fmudesign\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9825592-5952-4AB4-AD22-C7C9672DC6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEB3ECF-597F-4D14-932C-14F594BD30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="defaultvalues" sheetId="3" r:id="rId3"/>
     <sheet name="correlations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -158,7 +158,7 @@
  - beta(a, b, low, high)
  - pert(low, mode, high)
  - pert(low, mode, high, scale)
- - loguniform(low, high) [equivalent to exp(uniform(low, high))]
+ - loguniform(low, high) [equivalent to exp(uniform(log(low), log(high)))]
 </t>
         </r>
       </text>
@@ -856,7 +856,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -980,15 +980,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2089,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2110,58 +2105,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="70" t="s">
+      <c r="I1" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="71" t="s">
+      <c r="J1" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="72" t="s">
+      <c r="K1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="75" t="s">
+      <c r="O1" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="70" t="s">
+      <c r="P1" s="67" t="s">
         <v>24</v>
       </c>
       <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="73" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3"/>
@@ -2183,7 +2178,7 @@
       <c r="P2" s="13"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="74" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="14">
@@ -2203,11 +2198,11 @@
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
-      <c r="O3" s="61"/>
+      <c r="O3" s="58"/>
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="75" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="25">
@@ -2235,13 +2230,13 @@
       <c r="L4" s="33"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="63" t="s">
+      <c r="O4" s="60" t="s">
         <v>58</v>
       </c>
       <c r="P4" s="30"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="35"/>
       <c r="C5" s="56"/>
       <c r="D5" s="36" t="s">
@@ -2267,13 +2262,13 @@
         <v>1</v>
       </c>
       <c r="N5" s="42"/>
-      <c r="O5" s="62" t="s">
+      <c r="O5" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P5" s="39"/>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="35"/>
       <c r="C6" s="56"/>
       <c r="D6" s="36" t="s">
@@ -2295,13 +2290,13 @@
       <c r="L6" s="55"/>
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
-      <c r="O6" s="62" t="s">
+      <c r="O6" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P6" s="39"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="35"/>
       <c r="C7" s="56"/>
       <c r="D7" s="36" t="s">
@@ -2325,13 +2320,13 @@
       </c>
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
-      <c r="O7" s="62" t="s">
+      <c r="O7" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P7" s="39"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="79"/>
+      <c r="A8" s="76"/>
       <c r="B8" s="35"/>
       <c r="C8" s="56"/>
       <c r="D8" s="36" t="s">
@@ -2353,13 +2348,13 @@
       <c r="L8" s="55"/>
       <c r="M8" s="42"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="62" t="s">
+      <c r="O8" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P8" s="39"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="76"/>
       <c r="B9" s="35"/>
       <c r="C9" s="56"/>
       <c r="D9" s="36" t="s">
@@ -2381,13 +2376,13 @@
       <c r="L9" s="55"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
-      <c r="O9" s="62" t="s">
+      <c r="O9" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P9" s="39"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
+      <c r="A10" s="76"/>
       <c r="B10" s="35"/>
       <c r="C10" s="56"/>
       <c r="D10" s="36" t="s">
@@ -2413,13 +2408,13 @@
         <v>1</v>
       </c>
       <c r="N10" s="42"/>
-      <c r="O10" s="62" t="s">
+      <c r="O10" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P10" s="39"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
+      <c r="A11" s="76"/>
       <c r="B11" s="35"/>
       <c r="C11" s="56"/>
       <c r="D11" s="36" t="s">
@@ -2443,13 +2438,13 @@
       </c>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="62" t="s">
+      <c r="O11" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P11" s="39"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
+      <c r="A12" s="76"/>
       <c r="B12" s="35"/>
       <c r="C12" s="56"/>
       <c r="D12" s="36" t="s">
@@ -2475,13 +2470,13 @@
         <v>25</v>
       </c>
       <c r="N12" s="42"/>
-      <c r="O12" s="62" t="s">
+      <c r="O12" s="59" t="s">
         <v>58</v>
       </c>
       <c r="P12" s="39"/>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="80"/>
+      <c r="A13" s="77"/>
       <c r="B13" s="43"/>
       <c r="C13" s="44"/>
       <c r="D13" s="45" t="s">
@@ -2503,7 +2498,7 @@
       <c r="L13" s="51"/>
       <c r="M13" s="52"/>
       <c r="N13" s="52"/>
-      <c r="O13" s="81" t="s">
+      <c r="O13" s="78" t="s">
         <v>58</v>
       </c>
       <c r="P13" s="48"/>
@@ -2627,9 +2622,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2648,11 +2643,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" t="s">
         <v>36</v>
       </c>
       <c r="D1" t="s">
@@ -2681,279 +2675,264 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="59">
+      <c r="B2" s="57">
         <v>1</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="59">
+      <c r="C3" s="57">
         <v>1</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="60">
+      <c r="D4" s="57">
         <v>1</v>
       </c>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="58" t="s">
+      <c r="A5" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="59" t="s">
+      <c r="C5" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="59" t="s">
+      <c r="D5" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="57">
         <v>1</v>
       </c>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="F6" s="60">
+      <c r="F6" s="57">
         <v>1</v>
       </c>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="58" t="s">
+      <c r="A7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="59" t="s">
+      <c r="F7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="60">
+      <c r="G7" s="57">
         <v>1</v>
       </c>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="60" t="s">
+      <c r="D8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="60" t="s">
+      <c r="E8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="60" t="s">
+      <c r="F8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="60" t="s">
+      <c r="G8" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="60">
+      <c r="H8" s="57">
         <v>1</v>
       </c>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+      <c r="K8" s="57"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="59" t="s">
+      <c r="F9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G9" s="59" t="s">
+      <c r="G9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="59" t="s">
+      <c r="H9" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="57">
         <v>1</v>
       </c>
-      <c r="J9" s="60"/>
-      <c r="K9" s="60"/>
+      <c r="J9" s="57"/>
+      <c r="K9" s="57"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="58" t="s">
+      <c r="A10" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="59" t="s">
+      <c r="D10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="59" t="s">
+      <c r="F10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="H10" s="59" t="s">
+      <c r="H10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="I10" s="59" t="s">
+      <c r="I10" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="J10" s="60">
+      <c r="J10" s="57">
         <v>1</v>
       </c>
-      <c r="K10" s="60"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="60" t="s">
+      <c r="D11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="60" t="s">
+      <c r="E11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="60" t="s">
+      <c r="G11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="60" t="s">
+      <c r="H11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="60" t="s">
+      <c r="I11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="60" t="s">
+      <c r="J11" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="K11" s="60">
+      <c r="K11" s="57">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="57"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="57"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="57"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57"/>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Add dicrete and constant to examples
</commit_message>
<xml_diff>
--- a/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
+++ b/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\src\semeio\fmudesign\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEB3ECF-597F-4D14-932C-14F594BD30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DF84E-5F5D-5045-A375-59298AA99378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65780" yWindow="5960" windowWidth="39160" windowHeight="22160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="defaultvalues" sheetId="3" r:id="rId3"/>
     <sheet name="correlations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -149,16 +149,149 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">These are the distributions available.
- - normal(mean, std)
- - normal(mean, std, trunc_low, trunc_high)
- - uniform(low, high)
- - triangular(low, mode, high)
- - lognormal(mean, std) [equivalent to exp(normal(mean, std))]
- - beta(a, b)
- - beta(a, b, low, high)
- - pert(low, mode, high)
- - pert(low, mode, high, scale)
- - loguniform(low, high) [equivalent to exp(uniform(log(low), log(high)))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - normal(mean, std)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - normal(mean, std, trunc_low, trunc_high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - uniform(low, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - triangular(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - lognormal(mean, std) [equivalent to exp(normal(mean, std))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - beta(a, b)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - beta(a, b, low, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - pert(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - pert(low, mode, high, scale)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - loguniform(low, high) [equivalent to exp(uniform(log(low), log(high)))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - discrete([value1, value2, ..., value_n],[weight1, weight2, ..., weight_n])
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - constant(value)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -168,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>designtype</t>
   </si>
@@ -254,9 +387,6 @@
     <t>ref</t>
   </si>
   <si>
-    <t>montecarlo</t>
-  </si>
-  <si>
     <t>dist</t>
   </si>
   <si>
@@ -345,6 +475,33 @@
   </si>
   <si>
     <t>correlations</t>
+  </si>
+  <si>
+    <t>DISCRETE</t>
+  </si>
+  <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>CONSTANT</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>montecarlo1</t>
+  </si>
+  <si>
+    <t>montecarlo2</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
+  </si>
+  <si>
+    <t>defaultvalue</t>
+  </si>
+  <si>
+    <t>0.35,0.25,0.4</t>
   </si>
 </sst>
 </file>
@@ -394,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -725,30 +882,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -849,6 +982,19 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -955,23 +1101,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -988,8 +1131,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1015,15 +1158,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,8 +1500,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1409,8 +1557,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1466,8 +1614,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1523,8 +1671,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1580,8 +1728,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -2017,14 +2165,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="3" max="3" width="77.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2212,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2082,81 +2230,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="8" width="11.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
-    <col min="11" max="14" width="11.85546875" style="2" customWidth="1"/>
-    <col min="15" max="17" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" customWidth="1"/>
+    <col min="6" max="8" width="11.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="2" customWidth="1"/>
+    <col min="12" max="14" width="11.83203125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="11.83203125" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="72" t="s">
+      <c r="O1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="64" t="s">
         <v>24</v>
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="70" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3"/>
@@ -2177,8 +2326,8 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="71" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="14">
@@ -2198,28 +2347,28 @@
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
-      <c r="O3" s="58"/>
+      <c r="O3" s="55"/>
       <c r="P3" s="24"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
-        <v>28</v>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="72" t="s">
+        <v>62</v>
       </c>
       <c r="B4" s="25">
         <v>200</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>30</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="29"/>
       <c r="I4" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="31">
         <v>0</v>
@@ -2230,24 +2379,24 @@
       <c r="L4" s="33"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="60" t="s">
-        <v>58</v>
+      <c r="O4" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="P4" s="30"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="73"/>
       <c r="B5" s="35"/>
-      <c r="C5" s="56"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
       <c r="H5" s="38"/>
       <c r="I5" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="40">
         <v>0</v>
@@ -2255,31 +2404,31 @@
       <c r="K5" s="41">
         <v>1</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="52">
         <v>-1</v>
       </c>
       <c r="M5" s="42">
         <v>1</v>
       </c>
       <c r="N5" s="42"/>
-      <c r="O5" s="59" t="s">
-        <v>58</v>
+      <c r="O5" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P5" s="39"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="73"/>
       <c r="B6" s="35"/>
-      <c r="C6" s="56"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="35"/>
       <c r="G6" s="35"/>
       <c r="H6" s="38"/>
       <c r="I6" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="40">
         <v>-2</v>
@@ -2287,27 +2436,27 @@
       <c r="K6" s="41">
         <v>2</v>
       </c>
-      <c r="L6" s="55"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
-      <c r="O6" s="59" t="s">
-        <v>58</v>
+      <c r="O6" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P6" s="39"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="73"/>
       <c r="B7" s="35"/>
-      <c r="C7" s="56"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="38"/>
       <c r="I7" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="40">
         <v>-5</v>
@@ -2315,29 +2464,29 @@
       <c r="K7" s="41">
         <v>2</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="52">
         <v>5</v>
       </c>
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
-      <c r="O7" s="59" t="s">
-        <v>58</v>
+      <c r="O7" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P7" s="39"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="73"/>
       <c r="B8" s="35"/>
-      <c r="C8" s="56"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="38"/>
       <c r="I8" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="40">
         <v>0</v>
@@ -2345,27 +2494,27 @@
       <c r="K8" s="41">
         <v>1</v>
       </c>
-      <c r="L8" s="55"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="42"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="59" t="s">
-        <v>58</v>
+      <c r="O8" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P8" s="39"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="73"/>
       <c r="B9" s="35"/>
-      <c r="C9" s="56"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="38"/>
       <c r="I9" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="40">
         <v>2</v>
@@ -2373,27 +2522,27 @@
       <c r="K9" s="41">
         <v>5</v>
       </c>
-      <c r="L9" s="55"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
-      <c r="O9" s="59" t="s">
-        <v>58</v>
+      <c r="O9" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P9" s="39"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="73"/>
       <c r="B10" s="35"/>
-      <c r="C10" s="56"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="H10" s="38"/>
       <c r="I10" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="40">
         <v>4</v>
@@ -2401,31 +2550,31 @@
       <c r="K10" s="41">
         <v>2</v>
       </c>
-      <c r="L10" s="55">
+      <c r="L10" s="52">
         <v>-3</v>
       </c>
       <c r="M10" s="42">
         <v>1</v>
       </c>
       <c r="N10" s="42"/>
-      <c r="O10" s="59" t="s">
-        <v>58</v>
+      <c r="O10" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P10" s="39"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="73"/>
       <c r="B11" s="35"/>
-      <c r="C11" s="56"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="38"/>
       <c r="I11" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="40">
         <v>-3</v>
@@ -2433,29 +2582,29 @@
       <c r="K11" s="41">
         <v>1</v>
       </c>
-      <c r="L11" s="55">
+      <c r="L11" s="52">
         <v>4</v>
       </c>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="59" t="s">
-        <v>58</v>
+      <c r="O11" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P11" s="39"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="73"/>
       <c r="B12" s="35"/>
-      <c r="C12" s="56"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="38"/>
       <c r="I12" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="40">
         <v>-3</v>
@@ -2463,45 +2612,107 @@
       <c r="K12" s="41">
         <v>1</v>
       </c>
-      <c r="L12" s="55">
+      <c r="L12" s="52">
         <v>4</v>
       </c>
       <c r="M12" s="42">
         <v>25</v>
       </c>
       <c r="N12" s="42"/>
-      <c r="O12" s="59" t="s">
-        <v>58</v>
+      <c r="O12" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P12" s="39"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="46"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="53"/>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="49">
+      <c r="H13" s="44"/>
+      <c r="I13" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="46">
         <v>1</v>
       </c>
-      <c r="K13" s="50">
+      <c r="K13" s="47">
         <v>10</v>
       </c>
-      <c r="L13" s="51"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="78" t="s">
+      <c r="L13" s="48"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="75">
+        <v>200</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="P13" s="48"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="43">
+        <v>1</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="43">
+        <v>1</v>
+      </c>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2513,104 +2724,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2628,309 +2855,309 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="54">
+        <v>1</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="54">
+        <v>1</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="54">
+        <v>1</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="54">
+        <v>1</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="C7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="54">
+        <v>1</v>
+      </c>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="54">
+        <v>1</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="54">
+        <v>1</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="54">
+        <v>1</v>
+      </c>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="57">
-        <v>1</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="57">
-        <v>1</v>
-      </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="57">
-        <v>1</v>
-      </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="57">
-        <v>1</v>
-      </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="57">
-        <v>1</v>
-      </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="57">
-        <v>1</v>
-      </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="57">
-        <v>1</v>
-      </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="57">
-        <v>1</v>
-      </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="57">
-        <v>1</v>
-      </c>
-      <c r="K10" s="57"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="57">
+      <c r="B11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="54">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add pdfs to plots
</commit_message>
<xml_diff>
--- a/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
+++ b/src/semeio/fmudesign/examples/fmudesign_ex_montecarlo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Appl\github\semeio\src\semeio\fmudesign\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LGAZ/semeio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FEB3ECF-597F-4D14-932C-14F594BD30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DF84E-5F5D-5045-A375-59298AA99378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65780" yWindow="5960" windowWidth="39160" windowHeight="22160" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="defaultvalues" sheetId="3" r:id="rId3"/>
     <sheet name="correlations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -149,16 +149,149 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">These are the distributions available.
- - normal(mean, std)
- - normal(mean, std, trunc_low, trunc_high)
- - uniform(low, high)
- - triangular(low, mode, high)
- - lognormal(mean, std) [equivalent to exp(normal(mean, std))]
- - beta(a, b)
- - beta(a, b, low, high)
- - pert(low, mode, high)
- - pert(low, mode, high, scale)
- - loguniform(low, high) [equivalent to exp(uniform(log(low), log(high)))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - normal(mean, std)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - normal(mean, std, trunc_low, trunc_high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - uniform(low, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - triangular(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - lognormal(mean, std) [equivalent to exp(normal(mean, std))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - beta(a, b)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - beta(a, b, low, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - pert(low, mode, high)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - pert(low, mode, high, scale)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - loguniform(low, high) [equivalent to exp(uniform(log(low), log(high)))]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - discrete([value1, value2, ..., value_n],[weight1, weight2, ..., weight_n])
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve"> - constant(value)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -168,7 +301,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>designtype</t>
   </si>
@@ -254,9 +387,6 @@
     <t>ref</t>
   </si>
   <si>
-    <t>montecarlo</t>
-  </si>
-  <si>
     <t>dist</t>
   </si>
   <si>
@@ -345,6 +475,33 @@
   </si>
   <si>
     <t>correlations</t>
+  </si>
+  <si>
+    <t>DISCRETE</t>
+  </si>
+  <si>
+    <t>discrete</t>
+  </si>
+  <si>
+    <t>CONSTANT</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>montecarlo1</t>
+  </si>
+  <si>
+    <t>montecarlo2</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
+  </si>
+  <si>
+    <t>defaultvalue</t>
+  </si>
+  <si>
+    <t>0.35,0.25,0.4</t>
   </si>
 </sst>
 </file>
@@ -394,7 +551,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -725,30 +882,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -849,6 +982,19 @@
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -955,23 +1101,20 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -988,8 +1131,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1015,15 +1158,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1352,8 +1500,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1409,8 +1557,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1466,8 +1614,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1523,8 +1671,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -1580,8 +1728,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>405164</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>808060</xdr:colOff>
       <xdr:row>67</xdr:row>
       <xdr:rowOff>72720</xdr:rowOff>
     </xdr:to>
@@ -2017,14 +2165,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="77.85546875" customWidth="1"/>
+    <col min="3" max="3" width="77.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2032,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2040,7 +2188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2048,7 +2196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2056,7 +2204,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2064,7 +2212,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -2082,81 +2230,82 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" customWidth="1"/>
-    <col min="6" max="8" width="11.85546875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="2" customWidth="1"/>
-    <col min="11" max="14" width="11.85546875" style="2" customWidth="1"/>
-    <col min="15" max="17" width="11.85546875" customWidth="1"/>
-    <col min="20" max="20" width="9.85546875" customWidth="1"/>
-    <col min="22" max="22" width="9.85546875" customWidth="1"/>
+    <col min="6" max="8" width="11.83203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="10" max="10" width="33.1640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="2" customWidth="1"/>
+    <col min="12" max="14" width="11.83203125" style="2" customWidth="1"/>
+    <col min="15" max="17" width="11.83203125" customWidth="1"/>
+    <col min="20" max="20" width="9.83203125" customWidth="1"/>
+    <col min="22" max="22" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="61" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="65" t="s">
+      <c r="G1" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="66" t="s">
+      <c r="H1" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="67" t="s">
+      <c r="I1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="J1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="69" t="s">
+      <c r="K1" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="70" t="s">
+      <c r="L1" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="71" t="s">
+      <c r="M1" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="72" t="s">
+      <c r="O1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="64" t="s">
         <v>24</v>
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="73" t="s">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="70" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="3"/>
@@ -2177,8 +2326,8 @@
       <c r="O2" s="13"/>
       <c r="P2" s="13"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="74" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="71" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="14">
@@ -2198,28 +2347,28 @@
       <c r="L3" s="22"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
-      <c r="O3" s="58"/>
+      <c r="O3" s="55"/>
       <c r="P3" s="24"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="75" t="s">
-        <v>28</v>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="72" t="s">
+        <v>62</v>
       </c>
       <c r="B4" s="25">
         <v>200</v>
       </c>
       <c r="C4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>30</v>
       </c>
       <c r="E4" s="28"/>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
       <c r="H4" s="29"/>
       <c r="I4" s="30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="31">
         <v>0</v>
@@ -2230,24 +2379,24 @@
       <c r="L4" s="33"/>
       <c r="M4" s="34"/>
       <c r="N4" s="34"/>
-      <c r="O4" s="60" t="s">
-        <v>58</v>
+      <c r="O4" s="57" t="s">
+        <v>57</v>
       </c>
       <c r="P4" s="30"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="73"/>
       <c r="B5" s="35"/>
-      <c r="C5" s="56"/>
+      <c r="C5" s="53"/>
       <c r="D5" s="36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="37"/>
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
       <c r="H5" s="38"/>
       <c r="I5" s="39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="40">
         <v>0</v>
@@ -2255,31 +2404,31 @@
       <c r="K5" s="41">
         <v>1</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="52">
         <v>-1</v>
       </c>
       <c r="M5" s="42">
         <v>1</v>
       </c>
       <c r="N5" s="42"/>
-      <c r="O5" s="59" t="s">
-        <v>58</v>
+      <c r="O5" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P5" s="39"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="73"/>
       <c r="B6" s="35"/>
-      <c r="C6" s="56"/>
+      <c r="C6" s="53"/>
       <c r="D6" s="36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="37"/>
       <c r="F6" s="35"/>
       <c r="G6" s="35"/>
       <c r="H6" s="38"/>
       <c r="I6" s="39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="40">
         <v>-2</v>
@@ -2287,27 +2436,27 @@
       <c r="K6" s="41">
         <v>2</v>
       </c>
-      <c r="L6" s="55"/>
+      <c r="L6" s="52"/>
       <c r="M6" s="42"/>
       <c r="N6" s="42"/>
-      <c r="O6" s="59" t="s">
-        <v>58</v>
+      <c r="O6" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P6" s="39"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="73"/>
       <c r="B7" s="35"/>
-      <c r="C7" s="56"/>
+      <c r="C7" s="53"/>
       <c r="D7" s="36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="35"/>
       <c r="G7" s="35"/>
       <c r="H7" s="38"/>
       <c r="I7" s="39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="40">
         <v>-5</v>
@@ -2315,29 +2464,29 @@
       <c r="K7" s="41">
         <v>2</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="52">
         <v>5</v>
       </c>
       <c r="M7" s="42"/>
       <c r="N7" s="42"/>
-      <c r="O7" s="59" t="s">
-        <v>58</v>
+      <c r="O7" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P7" s="39"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="73"/>
       <c r="B8" s="35"/>
-      <c r="C8" s="56"/>
+      <c r="C8" s="53"/>
       <c r="D8" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E8" s="37"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="38"/>
       <c r="I8" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J8" s="40">
         <v>0</v>
@@ -2345,27 +2494,27 @@
       <c r="K8" s="41">
         <v>1</v>
       </c>
-      <c r="L8" s="55"/>
+      <c r="L8" s="52"/>
       <c r="M8" s="42"/>
       <c r="N8" s="42"/>
-      <c r="O8" s="59" t="s">
-        <v>58</v>
+      <c r="O8" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P8" s="39"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A9" s="73"/>
       <c r="B9" s="35"/>
-      <c r="C9" s="56"/>
+      <c r="C9" s="53"/>
       <c r="D9" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="37"/>
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="38"/>
       <c r="I9" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="40">
         <v>2</v>
@@ -2373,27 +2522,27 @@
       <c r="K9" s="41">
         <v>5</v>
       </c>
-      <c r="L9" s="55"/>
+      <c r="L9" s="52"/>
       <c r="M9" s="42"/>
       <c r="N9" s="42"/>
-      <c r="O9" s="59" t="s">
-        <v>58</v>
+      <c r="O9" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P9" s="39"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="76"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="73"/>
       <c r="B10" s="35"/>
-      <c r="C10" s="56"/>
+      <c r="C10" s="53"/>
       <c r="D10" s="36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="37"/>
       <c r="F10" s="35"/>
       <c r="G10" s="35"/>
       <c r="H10" s="38"/>
       <c r="I10" s="39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J10" s="40">
         <v>4</v>
@@ -2401,31 +2550,31 @@
       <c r="K10" s="41">
         <v>2</v>
       </c>
-      <c r="L10" s="55">
+      <c r="L10" s="52">
         <v>-3</v>
       </c>
       <c r="M10" s="42">
         <v>1</v>
       </c>
       <c r="N10" s="42"/>
-      <c r="O10" s="59" t="s">
-        <v>58</v>
+      <c r="O10" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P10" s="39"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" s="76"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A11" s="73"/>
       <c r="B11" s="35"/>
-      <c r="C11" s="56"/>
+      <c r="C11" s="53"/>
       <c r="D11" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E11" s="37"/>
       <c r="F11" s="35"/>
       <c r="G11" s="35"/>
       <c r="H11" s="38"/>
       <c r="I11" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="40">
         <v>-3</v>
@@ -2433,29 +2582,29 @@
       <c r="K11" s="41">
         <v>1</v>
       </c>
-      <c r="L11" s="55">
+      <c r="L11" s="52">
         <v>4</v>
       </c>
       <c r="M11" s="42"/>
       <c r="N11" s="42"/>
-      <c r="O11" s="59" t="s">
-        <v>58</v>
+      <c r="O11" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P11" s="39"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="76"/>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A12" s="73"/>
       <c r="B12" s="35"/>
-      <c r="C12" s="56"/>
+      <c r="C12" s="53"/>
       <c r="D12" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="37"/>
       <c r="F12" s="35"/>
       <c r="G12" s="35"/>
       <c r="H12" s="38"/>
       <c r="I12" s="39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="40">
         <v>-3</v>
@@ -2463,45 +2612,107 @@
       <c r="K12" s="41">
         <v>1</v>
       </c>
-      <c r="L12" s="55">
+      <c r="L12" s="52">
         <v>4</v>
       </c>
       <c r="M12" s="42">
         <v>25</v>
       </c>
       <c r="N12" s="42"/>
-      <c r="O12" s="59" t="s">
-        <v>58</v>
+      <c r="O12" s="56" t="s">
+        <v>57</v>
       </c>
       <c r="P12" s="39"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="46"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A13" s="73"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="53"/>
       <c r="F13" s="43"/>
       <c r="G13" s="43"/>
-      <c r="H13" s="47"/>
-      <c r="I13" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="J13" s="49">
+      <c r="H13" s="44"/>
+      <c r="I13" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="46">
         <v>1</v>
       </c>
-      <c r="K13" s="50">
+      <c r="K13" s="47">
         <v>10</v>
       </c>
-      <c r="L13" s="51"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="78" t="s">
+      <c r="L13" s="48"/>
+      <c r="M13" s="49"/>
+      <c r="N13" s="49"/>
+      <c r="O13" s="74" t="s">
+        <v>57</v>
+      </c>
+      <c r="P13" s="45"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A14" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="75">
+        <v>200</v>
+      </c>
+      <c r="C14" s="75" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="P13" s="48"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="39" t="s">
+        <v>59</v>
+      </c>
+      <c r="J14" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A15" s="75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="43">
+        <v>1</v>
+      </c>
+      <c r="C15" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="J15" s="43">
+        <v>1</v>
+      </c>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2513,104 +2724,120 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="53" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="51" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2628,309 +2855,309 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="54">
+        <v>1</v>
+      </c>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="54">
+        <v>1</v>
+      </c>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="54">
+        <v>1</v>
+      </c>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="54">
+        <v>1</v>
+      </c>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="54">
+        <v>1</v>
+      </c>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="C7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="54">
+        <v>1</v>
+      </c>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="54">
+        <v>1</v>
+      </c>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="54">
+        <v>1</v>
+      </c>
+      <c r="J9" s="54"/>
+      <c r="K9" s="54"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="54">
+        <v>1</v>
+      </c>
+      <c r="K10" s="54"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>48</v>
       </c>
-      <c r="K1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="57">
-        <v>1</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="57">
-        <v>1</v>
-      </c>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="57">
-        <v>1</v>
-      </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="57" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="57">
-        <v>1</v>
-      </c>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="57">
-        <v>1</v>
-      </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="57">
-        <v>1</v>
-      </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="H8" s="57">
-        <v>1</v>
-      </c>
-      <c r="I8" s="57"/>
-      <c r="J8" s="57"/>
-      <c r="K8" s="57"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-      <c r="B9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="I9" s="57">
-        <v>1</v>
-      </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="57">
-        <v>1</v>
-      </c>
-      <c r="K10" s="57"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="J11" s="57" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="57">
+      <c r="B11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="F11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="54">
         <v>1</v>
       </c>
     </row>

</xml_diff>